<commit_message>
clean: clean up calibration code, remove engel simulation.
</commit_message>
<xml_diff>
--- a/data/minimize.xlsx
+++ b/data/minimize.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiewagner/repos/lynch-syndrome/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340EDBCD-E70B-1840-AA6A-6CDD3B14E13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81507B19-6655-544E-9971-2AFF79687A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{8CF798CC-FA81-AC45-8483-047A30CF93A0}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="20540" windowHeight="18880" xr2:uid="{8CF798CC-FA81-AC45-8483-047A30CF93A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="32">
   <si>
     <t>lambda_NS</t>
   </si>
@@ -142,7 +142,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -182,6 +182,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -203,13 +216,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0748FD2F-EE11-DA42-B222-EA7FB958DBE6}">
-  <dimension ref="A1:R60"/>
+  <dimension ref="A1:R78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="I82" sqref="I82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1517,6 +1532,274 @@
       <c r="J60">
         <f t="shared" si="9"/>
         <v>0.32916159624932939</v>
+      </c>
+    </row>
+    <row r="64" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="E64" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J64" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K64" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L64" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D65" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" s="7">
+        <v>6.318E-2</v>
+      </c>
+      <c r="F65" s="7">
+        <v>8.3555000000000004E-2</v>
+      </c>
+      <c r="G65" s="7">
+        <v>0.16582</v>
+      </c>
+      <c r="H65" s="7">
+        <v>0.37735000000000002</v>
+      </c>
+      <c r="I65" s="7">
+        <v>1.7133860000000001</v>
+      </c>
+      <c r="J65" s="7">
+        <v>0.40323900000000001</v>
+      </c>
+      <c r="K65" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="L65" s="7">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="66" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D66" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" s="7">
+        <v>8.3482000000000001E-2</v>
+      </c>
+      <c r="F66" s="7">
+        <v>0.16685900000000001</v>
+      </c>
+      <c r="G66" s="7">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="H66" s="7">
+        <v>0.47298099999999998</v>
+      </c>
+      <c r="I66" s="7">
+        <v>0.85916599999999999</v>
+      </c>
+      <c r="J66" s="7">
+        <v>0.39696300000000001</v>
+      </c>
+      <c r="K66" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="L66" s="7">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="67" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D67" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="7">
+        <v>6.3056000000000001E-2</v>
+      </c>
+      <c r="F67" s="7">
+        <v>0.117505</v>
+      </c>
+      <c r="G67" s="7">
+        <v>0.21629100000000001</v>
+      </c>
+      <c r="H67" s="7">
+        <v>0.23469999999999999</v>
+      </c>
+      <c r="I67" s="7">
+        <v>0.58726800000000001</v>
+      </c>
+      <c r="J67" s="7">
+        <v>0.39990999999999999</v>
+      </c>
+      <c r="K67" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="L67" s="7">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="71" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="E71">
+        <f>1-EXP(-E65)</f>
+        <v>6.1225520926159183E-2</v>
+      </c>
+      <c r="F71">
+        <f t="shared" ref="F71:J71" si="10">1-EXP(-F65)</f>
+        <v>8.0159505947220655E-2</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="10"/>
+        <v>0.15280128376547386</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="10"/>
+        <v>0.31432395472238495</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="10"/>
+        <v>0.8197455833131112</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="10"/>
+        <v>0.3318476081823708</v>
+      </c>
+    </row>
+    <row r="72" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="E72">
+        <f t="shared" ref="E72:J72" si="11">1-EXP(-E66)</f>
+        <v>8.0092355140180205E-2</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="11"/>
+        <v>0.15368106610557064</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="11"/>
+        <v>0.2817948309594297</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="11"/>
+        <v>0.37685808923851405</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="11"/>
+        <v>0.57648485329821475</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="11"/>
+        <v>0.32764109754817605</v>
+      </c>
+    </row>
+    <row r="73" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="E73">
+        <f t="shared" ref="E73:J73" si="12">1-EXP(-E67)</f>
+        <v>6.1109105673157416E-2</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="12"/>
+        <v>0.11086393394499638</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="12"/>
+        <v>0.19449913298743893</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="12"/>
+        <v>0.20919194353712978</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="12"/>
+        <v>0.44415622253776832</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="12"/>
+        <v>0.32961962244533982</v>
+      </c>
+    </row>
+    <row r="75" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="E75" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I75" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D76" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" s="7">
+        <v>1.2881999999999999E-2</v>
+      </c>
+      <c r="F76" s="7">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="G76" s="7">
+        <v>7.6996999999999996E-2</v>
+      </c>
+      <c r="H76" s="7">
+        <v>0.115032</v>
+      </c>
+      <c r="I76" s="7">
+        <v>2.4799199999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D77" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E77" s="7">
+        <v>1.208E-2</v>
+      </c>
+      <c r="F77" s="7">
+        <v>0.44200400000000001</v>
+      </c>
+      <c r="G77" s="7">
+        <v>0.178013</v>
+      </c>
+      <c r="H77" s="7">
+        <v>0.10873099999999999</v>
+      </c>
+      <c r="I77" s="7">
+        <v>2.519126</v>
+      </c>
+    </row>
+    <row r="78" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D78" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="7">
+        <v>4.7809999999999997E-3</v>
+      </c>
+      <c r="F78" s="7">
+        <v>0.38400099999999998</v>
+      </c>
+      <c r="G78" s="7">
+        <v>9.4002000000000002E-2</v>
+      </c>
+      <c r="H78" s="7">
+        <v>4.5741999999999998E-2</v>
+      </c>
+      <c r="I78" s="7">
+        <v>2.5005630000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>